<commit_message>
update, multiple esim provider ids
</commit_message>
<xml_diff>
--- a/Skytronsystem/skytron_api/static/StockUpload.xlsx
+++ b/Skytronsystem/skytron_api/static/StockUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\THE LOGICBOX\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59C322EE-7179-48DD-9175-8654EF7CFA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FFF5C8-580C-47FB-A10F-9CFC8FD7199B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D0AB19E0-B29D-4663-843D-2660DBE7C963}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16080" xr2:uid="{D0AB19E0-B29D-4663-843D-2660DBE7C963}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>123456789012</t>
   </si>
@@ -81,9 +81,6 @@
     <t>esim_validity</t>
   </si>
   <si>
-    <t>esim_provider</t>
-  </si>
-  <si>
     <t>remarks</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>Provider2</t>
   </si>
   <si>
-    <t>ProviderName</t>
-  </si>
-  <si>
     <t>Someremarkshere</t>
   </si>
   <si>
@@ -112,9 +106,6 @@
   </si>
   <si>
     <t>Provider4</t>
-  </si>
-  <si>
-    <t>AnotherProvider</t>
   </si>
   <si>
     <t>Moreremarkshere</t>
@@ -477,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA243AE-2080-4012-B02B-C735788549C2}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,14 +484,13 @@
     <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
     <col min="7" max="10" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5703125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="12" width="19.5703125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
@@ -535,16 +525,13 @@
       <c r="L1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -553,10 +540,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>0</v>
@@ -574,18 +561,15 @@
         <v>45352</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
@@ -594,10 +578,10 @@
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>1</v>
@@ -615,18 +599,15 @@
         <v>45353</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -635,10 +616,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>1</v>
@@ -656,10 +637,7 @@
         <v>45353</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed issid, mergerd device stock and stock assignment
</commit_message>
<xml_diff>
--- a/Skytronsystem/skytron_api/static/StockUpload.xlsx
+++ b/Skytronsystem/skytron_api/static/StockUpload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\THE LOGICBOX\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FFF5C8-580C-47FB-A10F-9CFC8FD7199B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C5F81F-47D8-4D9A-B7F0-0FE9C1426D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16080" xr2:uid="{D0AB19E0-B29D-4663-843D-2660DBE7C963}"/>
+    <workbookView xWindow="4485" yWindow="4875" windowWidth="24405" windowHeight="10590" xr2:uid="{D0AB19E0-B29D-4663-843D-2660DBE7C963}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>123456789012</t>
   </si>
@@ -39,18 +39,6 @@
     <t>876543210987</t>
   </si>
   <si>
-    <t>1234567890123</t>
-  </si>
-  <si>
-    <t>2345678901234</t>
-  </si>
-  <si>
-    <t>9876543210123</t>
-  </si>
-  <si>
-    <t>8765432101234</t>
-  </si>
-  <si>
     <t>device_esn</t>
   </si>
   <si>
@@ -70,12 +58,6 @@
   </si>
   <si>
     <t>msisdn2</t>
-  </si>
-  <si>
-    <t>imsi1</t>
-  </si>
-  <si>
-    <t>imsi2</t>
   </si>
   <si>
     <t>esim_validity</t>
@@ -468,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA243AE-2080-4012-B02B-C735788549C2}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,56 +464,50 @@
     <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="10" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -540,10 +516,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>0</v>
@@ -551,25 +527,19 @@
       <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>4</v>
+      <c r="I2" s="2">
+        <v>45352</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="2">
-        <v>45352</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
@@ -578,10 +548,10 @@
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>1</v>
@@ -589,25 +559,19 @@
       <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>5</v>
+      <c r="I3" s="2">
+        <v>45353</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="2">
-        <v>45353</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -616,10 +580,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>1</v>
@@ -627,17 +591,11 @@
       <c r="H4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>5</v>
+      <c r="I4" s="2">
+        <v>45353</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="2">
-        <v>45353</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>